<commit_message>
Add params descriptions, refactor a bit
</commit_message>
<xml_diff>
--- a/locales.xlsx
+++ b/locales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\polyakov\Desktop\Файлы\github\PingLog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192DA88C-C9B6-4A5C-853F-5CB3EDA1DAF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAE6387A-4793-4339-974F-E6366E21ACBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D06D17B0-1947-46F5-AAC3-20BE5AFD972A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D06D17B0-1947-46F5-AAC3-20BE5AFD972A}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>$"Specifies the number of echo Request messages be sent. The default is {max_messages}. The maximum is 18,446,744,073,709,551,615."</t>
   </si>
@@ -108,9 +108,6 @@
     <t>s specified error</t>
   </si>
   <si>
-    <t>$"Key s specified, but file \"{source_file}\" is not exist. {Name} will ignore this key."</t>
-  </si>
-  <si>
     <t>$"{output} failed: {e.Message}"</t>
   </si>
   <si>
@@ -138,9 +135,6 @@
     <t>d specified error</t>
   </si>
   <si>
-    <t>$"Key d specified, but directory \"{destination_folder}\" is not exist. {Name} will ignore this key."</t>
-  </si>
-  <si>
     <t>$"Specifies IPv4 used to ping. This parameter is only required to identify the target host by name."</t>
   </si>
   <si>
@@ -225,10 +219,19 @@
     <t>$"Указан ключ t. Сообщения будут отправляться указанным узлам до прекращения. Для отображения статистики и продолжения проверки нажмите CTRL+BREAK (CTRL+\ под Linux). Для прекращения проверки, отображения статистики и выхода нажмите CTRL+C."</t>
   </si>
   <si>
-    <t>$"Specifies {Name} continue sending echo Request messages to the destination until interrupted. To display statistic and continue, press CTRL+BREAK (CTRL+\ on Linux). To interrupt, display statistics and quit, press CTRL+C. Will display message if specified."</t>
-  </si>
-  <si>
-    <t>$"Key t specified. {Name} will continue sending echo Request messages to the destination until interrupted. To display statistic and continue, press CTRL+BREAK (CTRL+\ on Linux). To interrupt, display statistics and quit, press CTRL+C."</t>
+    <t>$"Specifies {Name} continue sending echo Request messages to the destination until interrupted. To display statistic and continue, press CTRL+BREAK (CTRL+\\ on Linux). To interrupt, display statistics and quit, press CTRL+C. Will display message if specified."</t>
+  </si>
+  <si>
+    <t>$"Key t specified. {Name} will continue sending echo Request messages to the destination until interrupted. To display statistic and continue, press CTRL+BREAK (CTRL+\\ on Linux). To interrupt, display statistics and quit, press CTRL+C."</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>$"Key d specified, but directory \"{destination_folder}\" does not exist. {Name} will ignore this key."</t>
+  </si>
+  <si>
+    <t>$"Key s specified, but file \"{source_file}\" does not exist. {Name} will ignore this key."</t>
   </si>
 </sst>
 </file>
@@ -274,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -282,15 +285,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -306,9 +312,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -346,7 +352,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -452,7 +458,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -602,10 +608,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB8409ED-A9E7-4EA9-8D4E-0276BD8812C3}">
-  <dimension ref="A2:C25"/>
+  <dimension ref="A2:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,264 +621,318 @@
     <col min="3" max="3" width="117.85546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D2" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D3" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D6" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>6</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D14" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D15" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="D16" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D17" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="1" t="s">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B23" s="1" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3"/>
-      <c r="B25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>